<commit_message>
edit exam enrollment test analysis
</commit_message>
<xml_diff>
--- a/test-analysis.xlsx
+++ b/test-analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matej.LAPTOP-PB84M7CF\Documents\MFF\uvod-do-swi\uvod-sw-inz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{47E9AB93-309F-4148-B3E2-6562DB63E5B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA1D443-94CE-4A85-8E5E-4D84590352D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F23F0EAA-93EF-4F1B-859A-665DC19E58AD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="41">
   <si>
     <t>Title</t>
   </si>
@@ -93,6 +93,72 @@
   </si>
   <si>
     <t>Covered test conditions</t>
+  </si>
+  <si>
+    <t>TC_01</t>
+  </si>
+  <si>
+    <t>Student can sign up for an exam</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Student account available with enrolled courses and necessary permissions</t>
+  </si>
+  <si>
+    <t>xxx</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>Log into SIS as student</t>
+  </si>
+  <si>
+    <t>Open list of all exams of his enrolled courses</t>
+  </si>
+  <si>
+    <t>Enroll to the exam</t>
+  </si>
+  <si>
+    <t>Log in successful, home page displayed</t>
+  </si>
+  <si>
+    <t>List of all exams displayed</t>
+  </si>
+  <si>
+    <t>Detail displayed</t>
+  </si>
+  <si>
+    <t>Open detail of one exam with free spaces available</t>
+  </si>
+  <si>
+    <t>Student successfully enrolled</t>
+  </si>
+  <si>
+    <t>TC_02</t>
+  </si>
+  <si>
+    <t>Student can not sign up for an exam with full capacity</t>
+  </si>
+  <si>
+    <t>Open detail of one exam with no free spaces available</t>
+  </si>
+  <si>
+    <t>Try to enroll to the exam</t>
+  </si>
+  <si>
+    <t>Message displayed, option to sign up in the waiting line</t>
+  </si>
+  <si>
+    <t>5.</t>
+  </si>
+  <si>
+    <t>Sign up to the waiting line</t>
+  </si>
+  <si>
+    <t>Student successfully signed up to the waiting line</t>
   </si>
 </sst>
 </file>
@@ -631,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D6942B2-16F1-46ED-A992-15CA96840262}">
-  <dimension ref="B1:F15"/>
+  <dimension ref="B1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -651,7 +717,9 @@
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5"/>
+      <c r="C2" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="D2" s="6"/>
       <c r="E2" s="5"/>
       <c r="F2" s="7"/>
@@ -660,7 +728,9 @@
       <c r="B3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="22"/>
+      <c r="C3" s="22" t="s">
+        <v>20</v>
+      </c>
       <c r="D3" s="22"/>
       <c r="E3" s="20"/>
       <c r="F3" s="9"/>
@@ -669,32 +739,45 @@
       <c r="B4" s="8" t="s">
         <v>2</v>
       </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
       <c r="F4" s="10"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B5" s="8" t="s">
         <v>3</v>
       </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
       <c r="F5" s="10"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="21"/>
+      <c r="C6" s="21" t="s">
+        <v>23</v>
+      </c>
       <c r="F6" s="10"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B7" s="8" t="s">
         <v>15</v>
       </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
       <c r="F7" s="10"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="21"/>
+      <c r="C8" s="21" t="s">
+        <v>23</v>
+      </c>
       <c r="F8" s="10"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.35">
@@ -733,8 +816,12 @@
       <c r="B12" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="C12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="E12" s="2"/>
       <c r="F12" s="12"/>
     </row>
@@ -742,8 +829,12 @@
       <c r="B13" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+      <c r="C13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="E13" s="2"/>
       <c r="F13" s="12"/>
     </row>
@@ -751,8 +842,12 @@
       <c r="B14" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+      <c r="C14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="E14" s="2"/>
       <c r="F14" s="15"/>
     </row>
@@ -761,10 +856,10 @@
         <v>14</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="E15" s="18" t="s">
         <v>17</v>
@@ -773,9 +868,183 @@
         <v>17</v>
       </c>
     </row>
+    <row r="18" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B19" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B20" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="22"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="9"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B21" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="10"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B22" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22" s="10"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B23" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" s="10"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B24" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" t="s">
+        <v>24</v>
+      </c>
+      <c r="F24" s="10"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B25" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25" s="10"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B26" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" s="10"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B27" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="12"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B28" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B29" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" s="2"/>
+      <c r="F29" s="12"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B30" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30" s="2"/>
+      <c r="F30" s="12"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B31" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E31" s="2"/>
+      <c r="F31" s="15"/>
+    </row>
+    <row r="32" spans="2:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B32" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32" s="19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B33" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" s="19" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C20:D20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>